<commit_message>
rr Mon Nov  3 04:56:32 PM CET 2025
</commit_message>
<xml_diff>
--- a/public/routers/A1_Gestión_y_negociación_de_contratos_de_energía/A11_Hasta_50_kW/A112_Facturación_por_potencia.xlsx
+++ b/public/routers/A1_Gestión_y_negociación_de_contratos_de_energía/A11_Hasta_50_kW/A112_Facturación_por_potencia.xlsx
@@ -584,7 +584,7 @@
         <v>35</v>
       </c>
       <c r="C2" t="n">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
@@ -712,7 +712,7 @@
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="E7" t="n">
         <v>44</v>
@@ -762,7 +762,7 @@
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="E9" t="n">
         <v>45</v>
@@ -787,7 +787,7 @@
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="E10" t="n">
         <v>43</v>
@@ -859,7 +859,7 @@
         <v>23</v>
       </c>
       <c r="C13" t="n">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="D13" t="n">
         <v>0</v>

</xml_diff>